<commit_message>
remove some unwanted columns from BY YEAR tables
</commit_message>
<xml_diff>
--- a/output files/Number of robberies by year and dismissal status.xlsx
+++ b/output files/Number of robberies by year and dismissal status.xlsx
@@ -380,7 +380,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C8"/>
+  <dimension ref="A1:C9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -405,7 +405,7 @@
         <v>0</v>
       </c>
       <c r="C2">
-        <v>92</v>
+        <v>21</v>
       </c>
     </row>
     <row r="3" spans="1:3">
@@ -414,7 +414,7 @@
         <v>1</v>
       </c>
       <c r="C3">
-        <v>7</v>
+        <v>4</v>
       </c>
     </row>
     <row r="4" spans="1:3">
@@ -425,7 +425,7 @@
         <v>0</v>
       </c>
       <c r="C4">
-        <v>64</v>
+        <v>71</v>
       </c>
     </row>
     <row r="5" spans="1:3">
@@ -434,7 +434,7 @@
         <v>1</v>
       </c>
       <c r="C5">
-        <v>6</v>
+        <v>2</v>
       </c>
     </row>
     <row r="6" spans="1:3">
@@ -445,7 +445,7 @@
         <v>0</v>
       </c>
       <c r="C6">
-        <v>28</v>
+        <v>56</v>
       </c>
     </row>
     <row r="7" spans="1:3">
@@ -454,7 +454,7 @@
         <v>1</v>
       </c>
       <c r="C7">
-        <v>9</v>
+        <v>12</v>
       </c>
     </row>
     <row r="8" spans="1:3">
@@ -465,14 +465,24 @@
         <v>0</v>
       </c>
       <c r="C8">
-        <v>2</v>
+        <v>38</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3">
+      <c r="A9" s="1"/>
+      <c r="B9" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="C9">
+        <v>4</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="3">
+  <mergeCells count="4">
     <mergeCell ref="A2:A3"/>
     <mergeCell ref="A4:A5"/>
     <mergeCell ref="A6:A7"/>
+    <mergeCell ref="A8:A9"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>